<commit_message>
update the excel files
</commit_message>
<xml_diff>
--- a/assets/Districts.xlsx
+++ b/assets/Districts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\business_go\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haifam/Downloads/businessgo/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1C0CBB-BFD0-4C9A-9D6C-F70064C28A9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901A7D5D-20F4-634C-9D3D-E9B0178D2A78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1280" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1582,27 +1582,27 @@
   <dimension ref="A1:M209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>74483</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>16246</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>30889</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>36863</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>48929</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>7583</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>7195</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>21590</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>11266</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>102526</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>30361</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>38576</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>14809</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>7463</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>21332</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>30874</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>19403</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>21441</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>27025</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>19008</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>20257</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>12236</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>14807</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>16058</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>6407</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>29695</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>6709</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>5206</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>4134</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>7826</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>14102</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>28985</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>7656</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>12098</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>4882</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>10471</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>68832</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>2676</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>5952</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>6541</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>3801</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>3536</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>3841</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>52448</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>6563</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>14972</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>38333</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>33609</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>17291</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>49877</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>13265</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>101668</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>81557</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>27024</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>7114</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>21355</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>94332</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>93856</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>9254</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>18733</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>9435</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>4386</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>8123</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>18445</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>6718</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>5005</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>10666</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>35811</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>16279</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>5215</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>22718</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>76310</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>46331</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>4993</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>7569</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>14105</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>25055</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>3375</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>7615</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>20096</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>42837</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>23935</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>45298</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>45378</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>41717</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>57792</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>11790</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>5313</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>33716</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>42436</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>18353</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>2645</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>14236</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>16985</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>34872</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>7131</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>13123</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>72681</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>27196</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -6932,7 +6932,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>2174</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>4079</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -7260,7 +7260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -7301,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -7547,7 +7547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -7670,7 +7670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -7875,7 +7875,7 @@
         <v>13199</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -7916,7 +7916,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -7998,7 +7998,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -8039,7 +8039,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>39523</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -8121,7 +8121,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -8162,7 +8162,7 @@
         <v>34226</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>38659</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>29630</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -8285,7 +8285,7 @@
         <v>34560</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>109368</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -8367,7 +8367,7 @@
         <v>28028</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -8408,7 +8408,7 @@
         <v>31484</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -8449,7 +8449,7 @@
         <v>8144</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>1731</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>11992</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -8572,7 +8572,7 @@
         <v>1683</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -8613,7 +8613,7 @@
         <v>4754</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>3334</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -8695,7 +8695,7 @@
         <v>6507</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -8736,7 +8736,7 @@
         <v>27580</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -8777,7 +8777,7 @@
         <v>19968</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -8818,7 +8818,7 @@
         <v>36848</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>2798</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>15877</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>5694</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -8982,7 +8982,7 @@
         <v>8585</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -9023,7 +9023,7 @@
         <v>6569</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -9064,7 +9064,7 @@
         <v>20702</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -9105,7 +9105,7 @@
         <v>16570</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>22083</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>11062</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -9228,7 +9228,7 @@
         <v>13507</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -9269,7 +9269,7 @@
         <v>28911</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -9310,7 +9310,7 @@
         <v>16425</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -9351,7 +9351,7 @@
         <v>41598</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>20382</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -9433,7 +9433,7 @@
         <v>29881</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -9474,7 +9474,7 @@
         <v>42085</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -9515,7 +9515,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -9556,7 +9556,7 @@
         <v>34061</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
@@ -9597,7 +9597,7 @@
         <v>20267</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>16597</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -9679,7 +9679,7 @@
         <v>39681</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>23388</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
@@ -9761,7 +9761,7 @@
         <v>66785</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>199</v>
       </c>
@@ -9802,7 +9802,7 @@
         <v>14453</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
@@ -9843,7 +9843,7 @@
         <v>48258</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>201</v>
       </c>
@@ -9884,7 +9884,7 @@
         <v>17287</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>202</v>
       </c>
@@ -9925,7 +9925,7 @@
         <v>19016</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>203</v>
       </c>
@@ -9966,7 +9966,7 @@
         <v>14429</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>204</v>
       </c>
@@ -10007,7 +10007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>205</v>
       </c>
@@ -10048,7 +10048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>206</v>
       </c>
@@ -10089,7 +10089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>207</v>
       </c>
@@ -10130,7 +10130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>208</v>
       </c>

</xml_diff>